<commit_message>
14-11-2024 POC CatAndNonCat PR Create
</commit_message>
<xml_diff>
--- a/GePS-YIL/Downloads/NonCatalogPRItemsImport.xlsx
+++ b/GePS-YIL/Downloads/NonCatalogPRItemsImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\IdeaProjects\Cormsquare\GePS-YIL\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370481EF-A0EA-4DF0-9BF6-A45417AFA569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3416E5B-FDDE-4116-91C8-A8DBEE5D73E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6D71ECD4-D216-45FC-A56B-96951878AF7B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Quantity</t>
   </si>
@@ -52,118 +52,10 @@
     <t>ITM-05479</t>
   </si>
   <si>
-    <t>ITM-05480</t>
-  </si>
-  <si>
-    <t>ITM-05481</t>
-  </si>
-  <si>
-    <t>ITM-05482</t>
-  </si>
-  <si>
-    <t>ITM-05483</t>
-  </si>
-  <si>
-    <t>ITM-05484</t>
-  </si>
-  <si>
-    <t>ITM-05485</t>
-  </si>
-  <si>
-    <t>ITM-05486</t>
-  </si>
-  <si>
-    <t>ITM-05487</t>
-  </si>
-  <si>
-    <t>ITM-05488</t>
-  </si>
-  <si>
-    <t>ITM-05489</t>
-  </si>
-  <si>
-    <t>ITM-05490</t>
-  </si>
-  <si>
-    <t>ITM-05491</t>
-  </si>
-  <si>
-    <t>ITM-05492</t>
-  </si>
-  <si>
-    <t>ITM-05493</t>
-  </si>
-  <si>
-    <t>ITM-05494</t>
-  </si>
-  <si>
-    <t>ITM-05495</t>
-  </si>
-  <si>
-    <t>ITM-05496</t>
-  </si>
-  <si>
-    <t>ITM-05497</t>
-  </si>
-  <si>
     <t>Desc 2</t>
   </si>
   <si>
     <t>Desc 3</t>
-  </si>
-  <si>
-    <t>Desc 4</t>
-  </si>
-  <si>
-    <t>Desc 5</t>
-  </si>
-  <si>
-    <t>Desc 6</t>
-  </si>
-  <si>
-    <t>Desc 7</t>
-  </si>
-  <si>
-    <t>Desc 8</t>
-  </si>
-  <si>
-    <t>Desc 9</t>
-  </si>
-  <si>
-    <t>Desc 10</t>
-  </si>
-  <si>
-    <t>Desc 11</t>
-  </si>
-  <si>
-    <t>Desc 12</t>
-  </si>
-  <si>
-    <t>Desc 13</t>
-  </si>
-  <si>
-    <t>Desc 14</t>
-  </si>
-  <si>
-    <t>Desc 15</t>
-  </si>
-  <si>
-    <t>Desc 16</t>
-  </si>
-  <si>
-    <t>Desc 17</t>
-  </si>
-  <si>
-    <t>Desc 18</t>
-  </si>
-  <si>
-    <t>Desc 19</t>
-  </si>
-  <si>
-    <t>Desc 20</t>
-  </si>
-  <si>
-    <t>Desc 21</t>
   </si>
 </sst>
 </file>
@@ -530,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AE6AB4-276F-428D-925F-5FE060AD5DF2}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,7 +455,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -574,205 +466,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>